<commit_message>
Re - updated Test Cases
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS documents for Static Testing/ALS - Test Cases.xlsx
+++ b/documentation/quality/ALS documents for Static Testing/ALS - Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="629" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="629" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Documentation" sheetId="1" r:id="rId1"/>
@@ -2173,7 +2173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2269,17 +2269,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2319,17 +2313,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2358,23 +2358,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2385,32 +2370,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="132">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="129">
     <dxf>
       <fill>
         <patternFill>
@@ -4491,531 +4479,531 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="56"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="56"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="54"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="56"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="56"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="S24" s="56"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56"/>
-      <c r="S26" s="56"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="54"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -5075,43 +5063,43 @@
     </row>
     <row r="3" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="75"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="61" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="63"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="80"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="77"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
-      <c r="C5" s="57"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -5122,8 +5110,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
@@ -5145,10 +5133,10 @@
       <c r="D8" s="69"/>
       <c r="E8" s="69"/>
       <c r="F8" s="70"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="64"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
@@ -5675,41 +5663,41 @@
     </row>
     <row r="44" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="9"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="58" t="s">
+      <c r="C44" s="55"/>
+      <c r="D44" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="59"/>
-      <c r="F44" s="60"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="58"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="74" t="s">
+      <c r="H44" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="75"/>
+      <c r="I44" s="60"/>
       <c r="J44" s="16"/>
     </row>
     <row r="45" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="80" t="s">
+      <c r="C45" s="55"/>
+      <c r="D45" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="81"/>
-      <c r="F45" s="82"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="77"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="77"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="62"/>
       <c r="J45" s="17"/>
     </row>
     <row r="46" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="62"/>
-      <c r="F46" s="63"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="80"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="77"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="62"/>
       <c r="J46" s="10"/>
     </row>
     <row r="47" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5719,8 +5707,8 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="79"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="64"/>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5740,10 +5728,10 @@
       <c r="D49" s="69"/>
       <c r="E49" s="69"/>
       <c r="F49" s="70"/>
-      <c r="H49" s="64" t="s">
+      <c r="H49" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I49" s="64"/>
+      <c r="I49" s="74"/>
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5804,71 +5792,71 @@
     <row r="54" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H3:I6"/>
     <mergeCell ref="C44:C46"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="H44:I47"/>
     <mergeCell ref="C48:F52"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="D45:F46"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H3:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="131" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="19" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="20" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="128" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="16" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="17" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="18" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I41">
-    <cfRule type="containsText" dxfId="125" priority="13" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="122" priority="13" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="121" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="15" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="120" priority="15" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:I52">
-    <cfRule type="cellIs" dxfId="122" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="4" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:H52">
-    <cfRule type="cellIs" dxfId="119" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="1" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5887,8 +5875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5921,43 +5909,43 @@
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="75"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="80" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="77"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -5968,8 +5956,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
@@ -5991,10 +5979,10 @@
       <c r="D8" s="69"/>
       <c r="E8" s="69"/>
       <c r="F8" s="70"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="64"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
@@ -6420,41 +6408,41 @@
     </row>
     <row r="41" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58" t="s">
+      <c r="C41" s="55"/>
+      <c r="D41" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="74" t="s">
+      <c r="H41" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="75"/>
+      <c r="I41" s="60"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="80" t="s">
+      <c r="C42" s="55"/>
+      <c r="D42" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="81"/>
-      <c r="F42" s="82"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="77"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="77"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="63"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="77"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="62"/>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6464,8 +6452,8 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="79"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="64"/>
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6485,10 +6473,10 @@
       <c r="D46" s="69"/>
       <c r="E46" s="69"/>
       <c r="F46" s="70"/>
-      <c r="H46" s="64" t="s">
+      <c r="H46" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I46" s="64"/>
+      <c r="I46" s="74"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6550,71 +6538,71 @@
     <row r="51" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D4:F5"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="H41:I44"/>
     <mergeCell ref="C45:F49"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="D42:F43"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D4:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="116" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="13" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="113" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="10" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I38">
-    <cfRule type="containsText" dxfId="110" priority="7" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="107" priority="7" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="106" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="9" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="105" priority="9" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:I49">
-    <cfRule type="cellIs" dxfId="107" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="4" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47:H49">
-    <cfRule type="cellIs" dxfId="104" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="1" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6632,8 +6620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6666,43 +6654,43 @@
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="75"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="77"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -6713,8 +6701,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
@@ -6736,10 +6724,10 @@
       <c r="D8" s="69"/>
       <c r="E8" s="69"/>
       <c r="F8" s="70"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="64"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
@@ -7157,41 +7145,41 @@
     </row>
     <row r="39" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="9"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58" t="s">
+      <c r="C39" s="55"/>
+      <c r="D39" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="59"/>
-      <c r="F39" s="60"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="58"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="74" t="s">
+      <c r="H39" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I39" s="75"/>
+      <c r="I39" s="60"/>
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58" t="s">
+      <c r="C40" s="55"/>
+      <c r="D40" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="81"/>
-      <c r="F40" s="82"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="77"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="77"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="62"/>
       <c r="J40" s="16"/>
     </row>
     <row r="41" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="63"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="80"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="77"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="62"/>
       <c r="J41" s="17"/>
     </row>
     <row r="42" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7201,8 +7189,8 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="79"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="64"/>
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7222,10 +7210,10 @@
       <c r="D44" s="69"/>
       <c r="E44" s="69"/>
       <c r="F44" s="70"/>
-      <c r="H44" s="64" t="s">
+      <c r="H44" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="64"/>
+      <c r="I44" s="74"/>
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7287,71 +7275,71 @@
     <row r="49" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="H39:I42"/>
     <mergeCell ref="D40:F41"/>
     <mergeCell ref="C43:F47"/>
     <mergeCell ref="H44:I44"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="101" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="16" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="17" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="18" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="98" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="13" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I36">
-    <cfRule type="containsText" dxfId="95" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="92" priority="10" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="91" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="12" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="90" priority="12" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:I47">
-    <cfRule type="cellIs" dxfId="92" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="7" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:H47">
-    <cfRule type="cellIs" dxfId="89" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="4" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7370,7 +7358,7 @@
   <dimension ref="B1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7403,43 +7391,43 @@
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="75"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="77"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -7450,8 +7438,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
@@ -7473,10 +7461,10 @@
       <c r="D8" s="69"/>
       <c r="E8" s="69"/>
       <c r="F8" s="70"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="64"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
@@ -8044,41 +8032,41 @@
     </row>
     <row r="41" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58" t="s">
+      <c r="C41" s="55"/>
+      <c r="D41" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="74" t="s">
+      <c r="H41" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="75"/>
+      <c r="I41" s="60"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="58" t="s">
+      <c r="C42" s="55"/>
+      <c r="D42" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="81"/>
-      <c r="F42" s="82"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="77"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="77"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="63"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="77"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="62"/>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8088,8 +8076,8 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="79"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="64"/>
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8109,10 +8097,10 @@
       <c r="D46" s="69"/>
       <c r="E46" s="69"/>
       <c r="F46" s="70"/>
-      <c r="H46" s="64" t="s">
+      <c r="H46" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I46" s="64"/>
+      <c r="I46" s="74"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8174,148 +8162,148 @@
     <row r="51" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="H41:I44"/>
     <mergeCell ref="D42:F43"/>
     <mergeCell ref="C45:F49"/>
     <mergeCell ref="H46:I46"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="86" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="37" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="39" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="83" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="34" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="35" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I24 I38">
-    <cfRule type="containsText" dxfId="80" priority="31" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="77" priority="31" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="32" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="76" priority="32" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="33" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="75" priority="33" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:I49">
-    <cfRule type="cellIs" dxfId="77" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="29" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="30" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47:H49">
-    <cfRule type="cellIs" dxfId="74" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="25" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I33">
-    <cfRule type="containsText" dxfId="71" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="containsText" dxfId="68" priority="19" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="20" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="21" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="63" priority="21" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26 I28">
-    <cfRule type="containsText" dxfId="65" priority="16" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="62" priority="16" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="18" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="60" priority="18" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="58" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="57" priority="15" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="55" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="54" priority="9" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:I35">
-    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:I37">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I36)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8367,43 +8355,43 @@
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="75"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="77"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -8414,8 +8402,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
@@ -8437,10 +8425,10 @@
       <c r="D8" s="69"/>
       <c r="E8" s="69"/>
       <c r="F8" s="70"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="64"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
@@ -8543,7 +8531,7 @@
         <v>330</v>
       </c>
       <c r="D16" s="26"/>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="24" t="s">
         <v>341</v>
       </c>
       <c r="F16" s="26"/>
@@ -8554,7 +8542,7 @@
       </c>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="2:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
         <v>333</v>
       </c>
@@ -8562,7 +8550,7 @@
         <v>332</v>
       </c>
       <c r="D17" s="27"/>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="53" t="s">
         <v>331</v>
       </c>
       <c r="F17" s="26" t="s">
@@ -8585,7 +8573,7 @@
         <v>336</v>
       </c>
       <c r="D18" s="27"/>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="53" t="s">
         <v>331</v>
       </c>
       <c r="F18" s="26" t="s">
@@ -8608,7 +8596,7 @@
         <v>337</v>
       </c>
       <c r="D19" s="27"/>
-      <c r="E19" s="55" t="s">
+      <c r="E19" s="53" t="s">
         <v>331</v>
       </c>
       <c r="F19" s="26" t="s">
@@ -8623,7 +8611,7 @@
       </c>
       <c r="J19" s="19"/>
     </row>
-    <row r="20" spans="2:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>340</v>
       </c>
@@ -8631,7 +8619,7 @@
         <v>338</v>
       </c>
       <c r="D20" s="27"/>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="53" t="s">
         <v>331</v>
       </c>
       <c r="F20" s="26" t="s">
@@ -8654,7 +8642,7 @@
         <v>343</v>
       </c>
       <c r="D21" s="27"/>
-      <c r="E21" s="55" t="s">
+      <c r="E21" s="53" t="s">
         <v>331</v>
       </c>
       <c r="F21" s="27" t="s">
@@ -8870,41 +8858,41 @@
     </row>
     <row r="41" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58" t="s">
+      <c r="C41" s="55"/>
+      <c r="D41" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="74" t="s">
+      <c r="H41" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="75"/>
+      <c r="I41" s="60"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="58" t="s">
+      <c r="C42" s="55"/>
+      <c r="D42" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="81"/>
-      <c r="F42" s="82"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="77"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="77"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="63"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="77"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="62"/>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8914,8 +8902,8 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="79"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="64"/>
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8937,10 +8925,10 @@
       <c r="D46" s="69"/>
       <c r="E46" s="69"/>
       <c r="F46" s="70"/>
-      <c r="H46" s="64" t="s">
+      <c r="H46" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I46" s="64"/>
+      <c r="I46" s="74"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9002,71 +8990,71 @@
     <row r="51" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="H41:I44"/>
     <mergeCell ref="D42:F43"/>
     <mergeCell ref="C45:F49"/>
     <mergeCell ref="H46:I46"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="50" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I38">
-    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="40" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:I49">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47:H49">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9090,7 +9078,7 @@
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16:E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9123,43 +9111,43 @@
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="74" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="75"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="77"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -9170,8 +9158,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
@@ -9193,10 +9181,10 @@
       <c r="D8" s="69"/>
       <c r="E8" s="69"/>
       <c r="F8" s="70"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="64"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
@@ -9295,11 +9283,11 @@
       <c r="B16" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="51" t="s">
         <v>161</v>
       </c>
       <c r="D16" s="26"/>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="81" t="s">
         <v>160</v>
       </c>
       <c r="F16" s="27" t="s">
@@ -9320,7 +9308,7 @@
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="81" t="s">
         <v>165</v>
       </c>
       <c r="F17" s="26" t="s">
@@ -9341,7 +9329,7 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="26"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="26" t="s">
         <v>170</v>
       </c>
@@ -9360,7 +9348,7 @@
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="26" t="s">
         <v>171</v>
       </c>
@@ -9379,7 +9367,7 @@
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="E20" s="82"/>
       <c r="F20" s="27" t="s">
         <v>172</v>
       </c>
@@ -9398,7 +9386,7 @@
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="26"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="27" t="s">
         <v>169</v>
       </c>
@@ -9417,7 +9405,7 @@
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="27"/>
-      <c r="E22" s="26"/>
+      <c r="E22" s="81"/>
       <c r="F22" s="26" t="s">
         <v>173</v>
       </c>
@@ -9436,7 +9424,7 @@
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
+      <c r="E23" s="82"/>
       <c r="F23" s="26" t="s">
         <v>176</v>
       </c>
@@ -9455,7 +9443,7 @@
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
+      <c r="E24" s="82"/>
       <c r="F24" s="26" t="s">
         <v>177</v>
       </c>
@@ -9474,7 +9462,7 @@
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
+      <c r="E25" s="82"/>
       <c r="F25" s="26" t="s">
         <v>178</v>
       </c>
@@ -9495,7 +9483,7 @@
         <v>182</v>
       </c>
       <c r="D26" s="27"/>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="81" t="s">
         <v>160</v>
       </c>
       <c r="F26" s="27" t="s">
@@ -9514,7 +9502,7 @@
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
       <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
+      <c r="E27" s="82"/>
       <c r="F27" s="27" t="s">
         <v>186</v>
       </c>
@@ -9535,7 +9523,7 @@
         <v>188</v>
       </c>
       <c r="D28" s="27"/>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="82" t="s">
         <v>160</v>
       </c>
       <c r="F28" s="27" t="s">
@@ -9556,7 +9544,7 @@
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="E29" s="82"/>
       <c r="F29" s="27" t="s">
         <v>201</v>
       </c>
@@ -9575,7 +9563,7 @@
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="27"/>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="82" t="s">
         <v>205</v>
       </c>
       <c r="F30" s="27" t="s">
@@ -9598,7 +9586,7 @@
         <v>208</v>
       </c>
       <c r="D31" s="27"/>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="82" t="s">
         <v>211</v>
       </c>
       <c r="F31" s="27" t="s">
@@ -9619,7 +9607,7 @@
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
+      <c r="E32" s="82"/>
       <c r="F32" s="27" t="s">
         <v>213</v>
       </c>
@@ -9638,7 +9626,7 @@
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
+      <c r="E33" s="82"/>
       <c r="F33" s="27" t="s">
         <v>215</v>
       </c>
@@ -9659,7 +9647,7 @@
         <v>220</v>
       </c>
       <c r="D34" s="27"/>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="81" t="s">
         <v>221</v>
       </c>
       <c r="F34" s="27" t="s">
@@ -9680,7 +9668,7 @@
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
+      <c r="E35" s="82"/>
       <c r="F35" s="27" t="s">
         <v>186</v>
       </c>
@@ -9701,7 +9689,7 @@
         <v>226</v>
       </c>
       <c r="D36" s="27"/>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="82" t="s">
         <v>221</v>
       </c>
       <c r="F36" s="27" t="s">
@@ -9722,7 +9710,7 @@
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
+      <c r="E37" s="83"/>
       <c r="F37" s="36" t="s">
         <v>201</v>
       </c>
@@ -9742,13 +9730,13 @@
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="84" t="s">
         <v>258</v>
       </c>
       <c r="F38" s="41" t="s">
         <v>259</v>
       </c>
-      <c r="G38" s="52" t="s">
+      <c r="G38" s="50" t="s">
         <v>204</v>
       </c>
       <c r="H38" s="37"/>
@@ -9758,14 +9746,14 @@
       <c r="J38" s="37"/>
     </row>
     <row r="39" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="48" t="s">
         <v>229</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="D39" s="51"/>
-      <c r="E39" s="27" t="s">
+      <c r="D39" s="49"/>
+      <c r="E39" s="82" t="s">
         <v>221</v>
       </c>
       <c r="F39" s="27" t="s">
@@ -9781,14 +9769,14 @@
       <c r="J39" s="37"/>
     </row>
     <row r="40" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="52" t="s">
         <v>233</v>
       </c>
       <c r="C40" s="35" t="s">
         <v>277</v>
       </c>
-      <c r="D40" s="49"/>
-      <c r="E40" s="36" t="s">
+      <c r="D40" s="47"/>
+      <c r="E40" s="83" t="s">
         <v>278</v>
       </c>
       <c r="F40" s="36" t="s">
@@ -9797,11 +9785,11 @@
       <c r="G40" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H40" s="49"/>
-      <c r="I40" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J40" s="49"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="47"/>
     </row>
     <row r="41" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B41" s="42" t="s">
@@ -9809,7 +9797,7 @@
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="37"/>
-      <c r="E41" s="41"/>
+      <c r="E41" s="84"/>
       <c r="F41" s="41" t="s">
         <v>213</v>
       </c>
@@ -9817,18 +9805,18 @@
         <v>214</v>
       </c>
       <c r="H41" s="37"/>
-      <c r="I41" s="47" t="s">
+      <c r="I41" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J41" s="37"/>
     </row>
     <row r="42" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="52" t="s">
         <v>235</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="37"/>
-      <c r="E42" s="41"/>
+      <c r="E42" s="84"/>
       <c r="F42" s="41" t="s">
         <v>215</v>
       </c>
@@ -9836,20 +9824,20 @@
         <v>279</v>
       </c>
       <c r="H42" s="37"/>
-      <c r="I42" s="47" t="s">
+      <c r="I42" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="52" t="s">
         <v>240</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>232</v>
       </c>
       <c r="D43" s="26"/>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="81" t="s">
         <v>231</v>
       </c>
       <c r="F43" s="27" t="s">
@@ -9865,12 +9853,12 @@
       <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="52" t="s">
         <v>248</v>
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
+      <c r="E44" s="82"/>
       <c r="F44" s="27" t="s">
         <v>186</v>
       </c>
@@ -9884,14 +9872,14 @@
       <c r="J44" s="19"/>
     </row>
     <row r="45" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="52" t="s">
         <v>249</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>230</v>
       </c>
       <c r="D45" s="27"/>
-      <c r="E45" s="25" t="s">
+      <c r="E45" s="82" t="s">
         <v>231</v>
       </c>
       <c r="F45" s="36" t="s">
@@ -9907,14 +9895,14 @@
       <c r="J45" s="19"/>
     </row>
     <row r="46" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="52" t="s">
         <v>250</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="D46" s="51"/>
-      <c r="E46" s="27" t="s">
+      <c r="D46" s="49"/>
+      <c r="E46" s="82" t="s">
         <v>231</v>
       </c>
       <c r="F46" s="27" t="s">
@@ -9927,17 +9915,17 @@
       <c r="I46" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="J46" s="48"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="52" t="s">
         <v>260</v>
       </c>
       <c r="C47" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="D47" s="49"/>
-      <c r="E47" s="36" t="s">
+      <c r="D47" s="47"/>
+      <c r="E47" s="83" t="s">
         <v>287</v>
       </c>
       <c r="F47" s="36" t="s">
@@ -9946,19 +9934,19 @@
       <c r="G47" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H47" s="49"/>
-      <c r="I47" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J47" s="48"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J47" s="46"/>
     </row>
     <row r="48" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="52" t="s">
         <v>261</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="37"/>
-      <c r="E48" s="41"/>
+      <c r="E48" s="84"/>
       <c r="F48" s="41" t="s">
         <v>213</v>
       </c>
@@ -9966,18 +9954,18 @@
         <v>214</v>
       </c>
       <c r="H48" s="37"/>
-      <c r="I48" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J48" s="48"/>
+      <c r="I48" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J48" s="46"/>
     </row>
     <row r="49" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="52" t="s">
         <v>262</v>
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="37"/>
-      <c r="E49" s="41"/>
+      <c r="E49" s="84"/>
       <c r="F49" s="41" t="s">
         <v>215</v>
       </c>
@@ -9985,20 +9973,20 @@
         <v>288</v>
       </c>
       <c r="H49" s="37"/>
-      <c r="I49" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J49" s="48"/>
+      <c r="I49" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J49" s="46"/>
     </row>
     <row r="50" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="52" t="s">
         <v>263</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>241</v>
       </c>
       <c r="D50" s="27"/>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="81" t="s">
         <v>242</v>
       </c>
       <c r="F50" s="27" t="s">
@@ -10014,12 +10002,12 @@
       <c r="J50" s="40"/>
     </row>
     <row r="51" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="52" t="s">
         <v>264</v>
       </c>
       <c r="C51" s="25"/>
       <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
+      <c r="E51" s="82"/>
       <c r="F51" s="27" t="s">
         <v>186</v>
       </c>
@@ -10033,14 +10021,14 @@
       <c r="J51" s="40"/>
     </row>
     <row r="52" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="54" t="s">
+      <c r="B52" s="52" t="s">
         <v>272</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>245</v>
       </c>
       <c r="D52" s="27"/>
-      <c r="E52" s="27" t="s">
+      <c r="E52" s="82" t="s">
         <v>242</v>
       </c>
       <c r="F52" s="27" t="s">
@@ -10056,12 +10044,12 @@
       <c r="J52" s="40"/>
     </row>
     <row r="53" spans="2:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="52" t="s">
         <v>273</v>
       </c>
       <c r="C53" s="35"/>
       <c r="D53" s="36"/>
-      <c r="E53" s="27"/>
+      <c r="E53" s="82"/>
       <c r="F53" s="27" t="s">
         <v>201</v>
       </c>
@@ -10075,12 +10063,12 @@
       <c r="J53" s="40"/>
     </row>
     <row r="54" spans="2:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="B54" s="54" t="s">
+      <c r="B54" s="52" t="s">
         <v>274</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="37"/>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="85" t="s">
         <v>258</v>
       </c>
       <c r="F54" s="27" t="s">
@@ -10095,14 +10083,14 @@
       <c r="J54" s="40"/>
     </row>
     <row r="55" spans="2:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="54" t="s">
+      <c r="B55" s="52" t="s">
         <v>295</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="D55" s="51"/>
-      <c r="E55" s="27" t="s">
+      <c r="D55" s="49"/>
+      <c r="E55" s="82" t="s">
         <v>242</v>
       </c>
       <c r="F55" s="27" t="s">
@@ -10118,14 +10106,14 @@
       <c r="J55" s="40"/>
     </row>
     <row r="56" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B56" s="54" t="s">
+      <c r="B56" s="52" t="s">
         <v>296</v>
       </c>
       <c r="C56" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="D56" s="49"/>
-      <c r="E56" s="36" t="s">
+      <c r="D56" s="47"/>
+      <c r="E56" s="83" t="s">
         <v>293</v>
       </c>
       <c r="F56" s="36" t="s">
@@ -10134,19 +10122,19 @@
       <c r="G56" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H56" s="49"/>
-      <c r="I56" s="47" t="s">
+      <c r="H56" s="47"/>
+      <c r="I56" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J56" s="40"/>
     </row>
     <row r="57" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B57" s="54" t="s">
+      <c r="B57" s="52" t="s">
         <v>297</v>
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="37"/>
-      <c r="E57" s="41"/>
+      <c r="E57" s="84"/>
       <c r="F57" s="41" t="s">
         <v>213</v>
       </c>
@@ -10154,18 +10142,18 @@
         <v>214</v>
       </c>
       <c r="H57" s="37"/>
-      <c r="I57" s="47" t="s">
+      <c r="I57" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J57" s="40"/>
     </row>
     <row r="58" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="52" t="s">
         <v>298</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="37"/>
-      <c r="E58" s="41"/>
+      <c r="E58" s="84"/>
       <c r="F58" s="41" t="s">
         <v>215</v>
       </c>
@@ -10173,20 +10161,20 @@
         <v>294</v>
       </c>
       <c r="H58" s="37"/>
-      <c r="I58" s="47" t="s">
+      <c r="I58" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J58" s="40"/>
     </row>
     <row r="59" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="54" t="s">
+      <c r="B59" s="52" t="s">
         <v>299</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>251</v>
       </c>
       <c r="D59" s="27"/>
-      <c r="E59" s="24" t="s">
+      <c r="E59" s="81" t="s">
         <v>252</v>
       </c>
       <c r="F59" s="27" t="s">
@@ -10202,12 +10190,12 @@
       <c r="J59" s="40"/>
     </row>
     <row r="60" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B60" s="54" t="s">
+      <c r="B60" s="52" t="s">
         <v>300</v>
       </c>
       <c r="C60" s="25"/>
       <c r="D60" s="27"/>
-      <c r="E60" s="43"/>
+      <c r="E60" s="82"/>
       <c r="F60" s="27" t="s">
         <v>186</v>
       </c>
@@ -10221,14 +10209,14 @@
       <c r="J60" s="40"/>
     </row>
     <row r="61" spans="2:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="B61" s="54" t="s">
+      <c r="B61" s="52" t="s">
         <v>308</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>255</v>
       </c>
       <c r="D61" s="27"/>
-      <c r="E61" s="43" t="s">
+      <c r="E61" s="82" t="s">
         <v>252</v>
       </c>
       <c r="F61" s="27" t="s">
@@ -10244,12 +10232,12 @@
       <c r="J61" s="40"/>
     </row>
     <row r="62" spans="2:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="B62" s="54" t="s">
+      <c r="B62" s="52" t="s">
         <v>322</v>
       </c>
       <c r="C62" s="35"/>
       <c r="D62" s="36"/>
-      <c r="E62" s="43"/>
+      <c r="E62" s="82"/>
       <c r="F62" s="27" t="s">
         <v>201</v>
       </c>
@@ -10263,12 +10251,12 @@
       <c r="J62" s="40"/>
     </row>
     <row r="63" spans="2:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="54" t="s">
+      <c r="B63" s="52" t="s">
         <v>323</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37"/>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="85" t="s">
         <v>258</v>
       </c>
       <c r="F63" s="27" t="s">
@@ -10283,14 +10271,14 @@
       <c r="J63" s="40"/>
     </row>
     <row r="64" spans="2:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="52" t="s">
         <v>309</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="D64" s="51"/>
-      <c r="E64" s="27" t="s">
+      <c r="D64" s="49"/>
+      <c r="E64" s="82" t="s">
         <v>303</v>
       </c>
       <c r="F64" s="27" t="s">
@@ -10306,14 +10294,14 @@
       <c r="J64" s="40"/>
     </row>
     <row r="65" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B65" s="54" t="s">
+      <c r="B65" s="52" t="s">
         <v>310</v>
       </c>
       <c r="C65" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="D65" s="49"/>
-      <c r="E65" s="36" t="s">
+      <c r="D65" s="47"/>
+      <c r="E65" s="83" t="s">
         <v>304</v>
       </c>
       <c r="F65" s="36" t="s">
@@ -10322,19 +10310,19 @@
       <c r="G65" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H65" s="49"/>
-      <c r="I65" s="47" t="s">
+      <c r="H65" s="47"/>
+      <c r="I65" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J65" s="40"/>
     </row>
     <row r="66" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B66" s="54" t="s">
+      <c r="B66" s="52" t="s">
         <v>311</v>
       </c>
       <c r="C66" s="42"/>
       <c r="D66" s="37"/>
-      <c r="E66" s="41"/>
+      <c r="E66" s="84"/>
       <c r="F66" s="41" t="s">
         <v>213</v>
       </c>
@@ -10342,18 +10330,18 @@
         <v>214</v>
       </c>
       <c r="H66" s="37"/>
-      <c r="I66" s="47" t="s">
+      <c r="I66" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J66" s="40"/>
     </row>
     <row r="67" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="54" t="s">
+      <c r="B67" s="52" t="s">
         <v>324</v>
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="37"/>
-      <c r="E67" s="41"/>
+      <c r="E67" s="84"/>
       <c r="F67" s="41" t="s">
         <v>215</v>
       </c>
@@ -10361,20 +10349,20 @@
         <v>307</v>
       </c>
       <c r="H67" s="37"/>
-      <c r="I67" s="47" t="s">
+      <c r="I67" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J67" s="40"/>
     </row>
     <row r="68" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="54" t="s">
+      <c r="B68" s="52" t="s">
         <v>312</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>265</v>
       </c>
       <c r="D68" s="27"/>
-      <c r="E68" s="24" t="s">
+      <c r="E68" s="81" t="s">
         <v>266</v>
       </c>
       <c r="F68" s="27" t="s">
@@ -10390,12 +10378,12 @@
       <c r="J68" s="40"/>
     </row>
     <row r="69" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="52" t="s">
         <v>315</v>
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="27"/>
-      <c r="E69" s="43"/>
+      <c r="E69" s="82"/>
       <c r="F69" s="27" t="s">
         <v>186</v>
       </c>
@@ -10409,14 +10397,14 @@
       <c r="J69" s="40"/>
     </row>
     <row r="70" spans="2:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="52" t="s">
         <v>313</v>
       </c>
       <c r="C70" s="25" t="s">
         <v>269</v>
       </c>
       <c r="D70" s="27"/>
-      <c r="E70" s="43" t="s">
+      <c r="E70" s="82" t="s">
         <v>266</v>
       </c>
       <c r="F70" s="27" t="s">
@@ -10432,12 +10420,12 @@
       <c r="J70" s="40"/>
     </row>
     <row r="71" spans="2:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="52" t="s">
         <v>325</v>
       </c>
       <c r="C71" s="35"/>
       <c r="D71" s="36"/>
-      <c r="E71" s="46"/>
+      <c r="E71" s="83"/>
       <c r="F71" s="36" t="s">
         <v>201</v>
       </c>
@@ -10445,18 +10433,18 @@
         <v>202</v>
       </c>
       <c r="H71" s="36"/>
-      <c r="I71" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J71" s="45"/>
+      <c r="I71" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J71" s="44"/>
     </row>
     <row r="72" spans="2:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="B72" s="54" t="s">
+      <c r="B72" s="52" t="s">
         <v>326</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="37"/>
-      <c r="E72" s="41" t="s">
+      <c r="E72" s="84" t="s">
         <v>258</v>
       </c>
       <c r="F72" s="41" t="s">
@@ -10472,14 +10460,14 @@
       <c r="J72" s="37"/>
     </row>
     <row r="73" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B73" s="54" t="s">
+      <c r="B73" s="52" t="s">
         <v>314</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="D73" s="51"/>
-      <c r="E73" s="27" t="s">
+      <c r="D73" s="49"/>
+      <c r="E73" s="82" t="s">
         <v>266</v>
       </c>
       <c r="F73" s="27" t="s">
@@ -10495,14 +10483,14 @@
       <c r="J73" s="37"/>
     </row>
     <row r="74" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B74" s="54" t="s">
+      <c r="B74" s="52" t="s">
         <v>327</v>
       </c>
       <c r="C74" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="D74" s="49"/>
-      <c r="E74" s="36" t="s">
+      <c r="D74" s="47"/>
+      <c r="E74" s="83" t="s">
         <v>318</v>
       </c>
       <c r="F74" s="36" t="s">
@@ -10511,19 +10499,19 @@
       <c r="G74" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H74" s="49"/>
-      <c r="I74" s="47" t="s">
+      <c r="H74" s="47"/>
+      <c r="I74" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J74" s="37"/>
     </row>
     <row r="75" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="54" t="s">
+      <c r="B75" s="52" t="s">
         <v>328</v>
       </c>
       <c r="C75" s="42"/>
       <c r="D75" s="37"/>
-      <c r="E75" s="41"/>
+      <c r="E75" s="84"/>
       <c r="F75" s="41" t="s">
         <v>213</v>
       </c>
@@ -10531,18 +10519,18 @@
         <v>214</v>
       </c>
       <c r="H75" s="37"/>
-      <c r="I75" s="47" t="s">
+      <c r="I75" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J75" s="37"/>
     </row>
     <row r="76" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="54" t="s">
+      <c r="B76" s="52" t="s">
         <v>329</v>
       </c>
       <c r="C76" s="42"/>
       <c r="D76" s="37"/>
-      <c r="E76" s="41"/>
+      <c r="E76" s="84"/>
       <c r="F76" s="41" t="s">
         <v>215</v>
       </c>
@@ -10550,7 +10538,7 @@
         <v>321</v>
       </c>
       <c r="H76" s="37"/>
-      <c r="I76" s="47" t="s">
+      <c r="I76" s="45" t="s">
         <v>4</v>
       </c>
       <c r="J76" s="37"/>
@@ -10589,7 +10577,7 @@
       <c r="J79" s="37"/>
     </row>
     <row r="80" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="44"/>
+      <c r="B80" s="43"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="34"/>
@@ -10610,41 +10598,41 @@
     </row>
     <row r="82" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="9"/>
-      <c r="C82" s="57"/>
-      <c r="D82" s="58" t="s">
+      <c r="C82" s="55"/>
+      <c r="D82" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="59"/>
-      <c r="F82" s="60"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="58"/>
       <c r="G82" s="14"/>
-      <c r="H82" s="74" t="s">
+      <c r="H82" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I82" s="75"/>
+      <c r="I82" s="60"/>
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
-      <c r="C83" s="57"/>
-      <c r="D83" s="58" t="s">
+      <c r="C83" s="55"/>
+      <c r="D83" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E83" s="81"/>
-      <c r="F83" s="82"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="77"/>
       <c r="G83" s="3"/>
-      <c r="H83" s="76"/>
-      <c r="I83" s="77"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="62"/>
       <c r="J83" s="16"/>
     </row>
     <row r="84" spans="2:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="9"/>
-      <c r="C84" s="57"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="62"/>
-      <c r="F84" s="63"/>
+      <c r="C84" s="55"/>
+      <c r="D84" s="78"/>
+      <c r="E84" s="79"/>
+      <c r="F84" s="80"/>
       <c r="G84" s="5"/>
-      <c r="H84" s="76"/>
-      <c r="I84" s="77"/>
+      <c r="H84" s="61"/>
+      <c r="I84" s="62"/>
       <c r="J84" s="17"/>
     </row>
     <row r="85" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -10654,8 +10642,8 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="78"/>
-      <c r="I85" s="79"/>
+      <c r="H85" s="63"/>
+      <c r="I85" s="64"/>
       <c r="J85" s="10"/>
     </row>
     <row r="86" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -10675,10 +10663,10 @@
       <c r="D87" s="69"/>
       <c r="E87" s="69"/>
       <c r="F87" s="70"/>
-      <c r="H87" s="64" t="s">
+      <c r="H87" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="I87" s="64"/>
+      <c r="I87" s="74"/>
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10740,137 +10728,137 @@
     <row r="92" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="D82:F82"/>
     <mergeCell ref="H82:I85"/>
     <mergeCell ref="D83:F84"/>
     <mergeCell ref="C86:F90"/>
     <mergeCell ref="H87:I87"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I45 I50:I54">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I88:I90">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88:H90">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Not Run"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:I63">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I59)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68:I72 I77:I80">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:I49">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55:I58">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64:I67">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73:I76">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Not Run">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Not Run">
       <formula>NOT(ISERROR(SEARCH("Not Run",I73)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Modified Test Cases, added references
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS documents for Static Testing/ALS - Test Cases.xlsx
+++ b/documentation/quality/ALS documents for Static Testing/ALS - Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="629" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="629"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Documentation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="363">
   <si>
     <r>
       <rPr>
@@ -420,40 +420,6 @@
       </rPr>
       <t>READABILITY OF CALENDAR EVENTS (EVENT VIEW)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3.5 FUNCTIONAL TEST CASES FOR USE CASE: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>USABILITY OF CALENDAR LINKS (LINK REDIRECTION)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3.5 FUNCTIONAL TEST CASES FOR USE CASE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> USABILITY OF CALENDAR LINKS (LINK REDIRECTION)</t>
-    </r>
-  </si>
-  <si>
-    <t>Test Case validates the following: 
-• The links properly redirect the user to the necessary audio files / text files / websites</t>
   </si>
   <si>
     <t>3.5.1</t>
@@ -1749,6 +1715,49 @@
       </rPr>
       <t>Home page</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.5 FUNCTIONAL TEST CASES FOR USE CASE: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USABILITY OF CALENDAR (EVENT PLOTTING)</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Case validates the following: 
+• The Event Plotting of all movable feasts and the completeness of all the readings per month</t>
+  </si>
+  <si>
+    <t>Create Events</t>
+  </si>
+  <si>
+    <t>Read Events</t>
+  </si>
+  <si>
+    <t>Delete Events</t>
+  </si>
+  <si>
+    <t>Update Events</t>
+  </si>
+  <si>
+    <t>View Calendar Events/ Readings</t>
+  </si>
+  <si>
+    <t>View Calendar</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
   </si>
 </sst>
 </file>
@@ -2328,17 +2337,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2367,23 +2382,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2392,6 +2392,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4464,7 +4473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:S28"/>
     </sheetView>
   </sheetViews>
@@ -4475,12 +4484,12 @@
   <sheetData>
     <row r="2" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -5007,12 +5016,12 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -5029,8 +5038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5070,24 +5079,24 @@
       <c r="E3" s="62"/>
       <c r="F3" s="63"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="60"/>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="65"/>
-      <c r="F4" s="66"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
@@ -5098,8 +5107,8 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -5110,42 +5119,42 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="82"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
       <c r="J7" s="16"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73"/>
-      <c r="H8" s="67" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="H8" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="28">
         <f>COUNTIF(I16:I41,"Pass")/COUNTA(I16:I41)</f>
         <v>0</v>
@@ -5158,10 +5167,10 @@
     </row>
     <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="28">
         <f>COUNTIF(I16:I41,"Fail")/COUNTA(I16:I41)</f>
         <v>0</v>
@@ -5174,10 +5183,10 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="H11" s="28">
         <f>COUNTIF(I16:I41,"Not Run")/COUNTA(I16:I41)</f>
         <v>1</v>
@@ -5238,7 +5247,9 @@
       <c r="C16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="26" t="s">
+        <v>361</v>
+      </c>
       <c r="E16" s="26" t="s">
         <v>23</v>
       </c>
@@ -5261,7 +5272,9 @@
       <c r="C17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="27" t="s">
+        <v>362</v>
+      </c>
       <c r="E17" s="26" t="s">
         <v>23</v>
       </c>
@@ -5287,10 +5300,10 @@
         <v>29</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="24" t="s">
@@ -5306,10 +5319,10 @@
       <c r="D19" s="27"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="24" t="s">
@@ -5356,7 +5369,7 @@
     </row>
     <row r="22" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="27"/>
@@ -5375,7 +5388,7 @@
     </row>
     <row r="23" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="27"/>
@@ -5384,7 +5397,7 @@
         <v>46</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="24" t="s">
@@ -5399,7 +5412,9 @@
       <c r="C24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="27" t="s">
+        <v>361</v>
+      </c>
       <c r="E24" s="26" t="s">
         <v>23</v>
       </c>
@@ -5417,20 +5432,22 @@
     </row>
     <row r="25" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="27" t="s">
+        <v>361</v>
+      </c>
       <c r="E25" s="26" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H25" s="27"/>
       <c r="I25" s="24" t="s">
@@ -5508,7 +5525,7 @@
         <v>47</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H29" s="27"/>
       <c r="I29" s="24" t="s">
@@ -5670,34 +5687,34 @@
       <c r="E44" s="62"/>
       <c r="F44" s="63"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="77" t="s">
+      <c r="H44" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I44" s="78"/>
+      <c r="I44" s="65"/>
       <c r="J44" s="16"/>
     </row>
     <row r="45" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="60"/>
-      <c r="D45" s="83" t="s">
+      <c r="D45" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="84"/>
-      <c r="F45" s="85"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="82"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="80"/>
+      <c r="H45" s="66"/>
+      <c r="I45" s="67"/>
       <c r="J45" s="17"/>
     </row>
     <row r="46" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9"/>
       <c r="C46" s="60"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="66"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="85"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="80"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="67"/>
       <c r="J46" s="10"/>
     </row>
     <row r="47" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5707,39 +5724,39 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="81"/>
-      <c r="I47" s="82"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="69"/>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="9"/>
-      <c r="C48" s="68" t="s">
+      <c r="C48" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="69"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="70"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="72"/>
       <c r="G48" s="3"/>
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="9"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="73"/>
-      <c r="H49" s="67" t="s">
+      <c r="C49" s="73"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="75"/>
+      <c r="H49" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I49" s="67"/>
+      <c r="I49" s="79"/>
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="9"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="73"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="75"/>
       <c r="H50" s="28">
         <f>COUNTIF(I16:I41,"Pass")/COUNTA(I16:I41)</f>
         <v>0</v>
@@ -5751,10 +5768,10 @@
     </row>
     <row r="51" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="9"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="73"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="75"/>
       <c r="H51" s="28">
         <f>COUNTIF(I16:I41,"Fail")/COUNTA(I16:I41)</f>
         <v>0</v>
@@ -5766,10 +5783,10 @@
     </row>
     <row r="52" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="9"/>
-      <c r="C52" s="74"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="76"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="77"/>
+      <c r="E52" s="77"/>
+      <c r="F52" s="78"/>
       <c r="H52" s="28">
         <f>COUNTIF(I16:I41,"Not Run")/COUNTA(I16:I41)</f>
         <v>1</v>
@@ -5792,18 +5809,18 @@
     <row r="54" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H3:I6"/>
     <mergeCell ref="C44:C46"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="H44:I47"/>
     <mergeCell ref="C48:F52"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="D45:F46"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H3:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
     <cfRule type="cellIs" dxfId="128" priority="19" operator="equal">
@@ -5876,7 +5893,7 @@
   <dimension ref="B1:K51"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5916,36 +5933,36 @@
       <c r="E3" s="62"/>
       <c r="F3" s="63"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
       <c r="C4" s="60"/>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
       <c r="C5" s="60"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -5956,42 +5973,42 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="82"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
       <c r="J7" s="16"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73"/>
-      <c r="H8" s="67" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="H8" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="28">
         <f>COUNTIF(I16:I38,"Pass")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -6004,10 +6021,10 @@
     </row>
     <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="28">
         <f>COUNTIF(I16:I38,"Fail")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -6020,10 +6037,10 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="H11" s="28">
         <f>COUNTIF(I16:I38,"Not Run")/COUNTA(I16:I38)</f>
         <v>1</v>
@@ -6059,7 +6076,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>9</v>
@@ -6079,20 +6096,22 @@
     </row>
     <row r="16" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="F16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="24" t="s">
@@ -6102,18 +6121,20 @@
     </row>
     <row r="17" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="27"/>
+        <v>73</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E17" s="26"/>
       <c r="F17" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="24" t="s">
@@ -6123,18 +6144,18 @@
     </row>
     <row r="18" spans="2:10" ht="220.5" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="27"/>
       <c r="E18" s="26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="24" t="s">
@@ -6144,20 +6165,20 @@
     </row>
     <row r="19" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H19" s="32"/>
       <c r="I19" s="24" t="s">
@@ -6167,16 +6188,16 @@
     </row>
     <row r="20" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="27"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="24" t="s">
@@ -6186,20 +6207,20 @@
     </row>
     <row r="21" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="24" t="s">
@@ -6415,34 +6436,34 @@
       <c r="E41" s="62"/>
       <c r="F41" s="63"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="77" t="s">
+      <c r="H41" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="78"/>
+      <c r="I41" s="65"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
       <c r="C42" s="60"/>
-      <c r="D42" s="83" t="s">
+      <c r="D42" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="84"/>
-      <c r="F42" s="85"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="82"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="80"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="67"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
       <c r="C43" s="60"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="66"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="85"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="80"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="67"/>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6452,39 +6473,39 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="82"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="69"/>
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="9"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="72"/>
       <c r="G45" s="3"/>
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="73"/>
-      <c r="H46" s="67" t="s">
+      <c r="C46" s="73"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="75"/>
+      <c r="H46" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I46" s="67"/>
+      <c r="I46" s="79"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="73"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
       <c r="H47" s="28">
         <f>COUNTIF(I16:I38,"Pass")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -6496,10 +6517,10 @@
     </row>
     <row r="48" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="9"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="73"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="75"/>
       <c r="H48" s="28">
         <f>COUNTIF(I16:I38,"Fail")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -6511,10 +6532,10 @@
     </row>
     <row r="49" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="9"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="78"/>
       <c r="H49" s="28">
         <f>COUNTIF(I16:I38,"Not Run")/COUNTA(I16:I38)</f>
         <v>1</v>
@@ -6538,18 +6559,18 @@
     <row r="51" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D4:F5"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="H41:I44"/>
     <mergeCell ref="C45:F49"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="D42:F43"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D4:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
     <cfRule type="cellIs" dxfId="113" priority="13" operator="equal">
@@ -6620,8 +6641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K49"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A22" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6661,10 +6682,10 @@
       <c r="E3" s="62"/>
       <c r="F3" s="63"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
@@ -6674,23 +6695,23 @@
       <c r="D4" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
       <c r="C5" s="60"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -6701,42 +6722,42 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="82"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
       <c r="J7" s="16"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73"/>
-      <c r="H8" s="67" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="H8" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="28">
         <f>COUNTIF(I16:I36,"Pass")/COUNTA(I16:I36)</f>
         <v>0</v>
@@ -6749,10 +6770,10 @@
     </row>
     <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="28">
         <f>COUNTIF(I16:I36,"Fail")/COUNTA(I16:I36)</f>
         <v>0</v>
@@ -6765,10 +6786,10 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="H11" s="28">
         <f>COUNTIF(I16:I36,"Not Run")/COUNTA(I16:I36)</f>
         <v>1</v>
@@ -6827,17 +6848,19 @@
         <v>54</v>
       </c>
       <c r="C16" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="24" t="s">
@@ -6847,18 +6870,20 @@
     </row>
     <row r="17" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="27"/>
+        <v>73</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E17" s="26"/>
       <c r="F17" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="24" t="s">
@@ -6868,16 +6893,16 @@
     </row>
     <row r="18" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="27"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="24" t="s">
@@ -6887,20 +6912,22 @@
     </row>
     <row r="19" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="27"/>
+        <v>92</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E19" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="24" t="s">
@@ -6910,16 +6937,16 @@
     </row>
     <row r="20" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="27"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="24" t="s">
@@ -6929,16 +6956,16 @@
     </row>
     <row r="21" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="24" t="s">
@@ -6948,20 +6975,22 @@
     </row>
     <row r="22" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="27"/>
+        <v>101</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E22" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="24" t="s">
@@ -6971,16 +7000,16 @@
     </row>
     <row r="23" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="24" t="s">
@@ -7152,10 +7181,10 @@
       <c r="E39" s="62"/>
       <c r="F39" s="63"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="77" t="s">
+      <c r="H39" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I39" s="78"/>
+      <c r="I39" s="65"/>
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -7164,22 +7193,22 @@
       <c r="D40" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="84"/>
-      <c r="F40" s="85"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="80"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="67"/>
       <c r="J40" s="16"/>
     </row>
     <row r="41" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9"/>
       <c r="C41" s="60"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="66"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="85"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="80"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="67"/>
       <c r="J41" s="17"/>
     </row>
     <row r="42" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7189,39 +7218,39 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="82"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="69"/>
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
-      <c r="C43" s="68" t="s">
+      <c r="C43" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="70"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="72"/>
       <c r="G43" s="3"/>
       <c r="J43" s="16"/>
     </row>
     <row r="44" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="9"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="73"/>
-      <c r="H44" s="67" t="s">
+      <c r="C44" s="73"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="75"/>
+      <c r="H44" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="67"/>
+      <c r="I44" s="79"/>
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="9"/>
-      <c r="C45" s="71"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="73"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="75"/>
       <c r="H45" s="28">
         <f>COUNTIF(I16:I36,"Pass")/COUNTA(I16:I36)</f>
         <v>0</v>
@@ -7233,10 +7262,10 @@
     </row>
     <row r="46" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="75"/>
       <c r="H46" s="28">
         <f>COUNTIF(I16:I36,"Fail")/COUNTA(I16:I36)</f>
         <v>0</v>
@@ -7248,10 +7277,10 @@
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9"/>
-      <c r="C47" s="74"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="78"/>
       <c r="H47" s="28">
         <f>COUNTIF(I16:I36,"Not Run")/COUNTA(I16:I36)</f>
         <v>1</v>
@@ -7275,18 +7304,18 @@
     <row r="49" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="H39:I42"/>
     <mergeCell ref="D40:F41"/>
     <mergeCell ref="C43:F47"/>
     <mergeCell ref="H44:I44"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
     <cfRule type="cellIs" dxfId="98" priority="16" operator="equal">
@@ -7357,8 +7386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7398,10 +7427,10 @@
       <c r="E3" s="62"/>
       <c r="F3" s="63"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
@@ -7411,23 +7440,23 @@
       <c r="D4" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
       <c r="C5" s="60"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -7438,42 +7467,42 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="82"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
       <c r="J7" s="16"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73"/>
-      <c r="H8" s="67" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="H8" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="28">
         <f>COUNTIF(I16:I38,"Pass")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -7486,10 +7515,10 @@
     </row>
     <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="28">
         <f>COUNTIF(I16:I38,"Fail")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -7502,10 +7531,10 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="H11" s="28">
         <f>COUNTIF(I16:I38,"Not Run")/COUNTA(I16:I38)</f>
         <v>1</v>
@@ -7561,20 +7590,22 @@
     </row>
     <row r="16" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="24" t="s">
@@ -7584,18 +7615,20 @@
     </row>
     <row r="17" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="27"/>
+        <v>73</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>360</v>
+      </c>
       <c r="E17" s="26"/>
       <c r="F17" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="24" t="s">
@@ -7605,16 +7638,16 @@
     </row>
     <row r="18" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="27"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="24" t="s">
@@ -7624,20 +7657,22 @@
     </row>
     <row r="19" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="27"/>
+        <v>92</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E19" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="24" t="s">
@@ -7647,16 +7682,16 @@
     </row>
     <row r="20" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="27"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>100</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="24" t="s">
@@ -7666,16 +7701,16 @@
     </row>
     <row r="21" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="24" t="s">
@@ -7685,20 +7720,22 @@
     </row>
     <row r="22" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="27"/>
+        <v>110</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E22" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="24" t="s">
@@ -7708,16 +7745,16 @@
     </row>
     <row r="23" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="27"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="24" t="s">
@@ -7727,16 +7764,16 @@
     </row>
     <row r="24" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="24" t="s">
@@ -7746,20 +7783,22 @@
     </row>
     <row r="25" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="27"/>
+        <v>134</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E25" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H25" s="27"/>
       <c r="I25" s="24" t="s">
@@ -7769,16 +7808,16 @@
     </row>
     <row r="26" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B26" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="27"/>
       <c r="E26" s="26"/>
       <c r="F26" s="26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="24" t="s">
@@ -7788,16 +7827,16 @@
     </row>
     <row r="27" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H27" s="27"/>
       <c r="I27" s="24" t="s">
@@ -7807,16 +7846,16 @@
     </row>
     <row r="28" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="24" t="s">
@@ -7826,20 +7865,22 @@
     </row>
     <row r="29" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B29" s="24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="27"/>
+        <v>126</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E29" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H29" s="27"/>
       <c r="I29" s="24" t="s">
@@ -7849,18 +7890,18 @@
     </row>
     <row r="30" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="27"/>
       <c r="E30" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="24" t="s">
@@ -7870,16 +7911,16 @@
     </row>
     <row r="31" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="24" t="s">
@@ -7889,18 +7930,18 @@
     </row>
     <row r="32" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="27"/>
       <c r="E32" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="24" t="s">
@@ -7910,16 +7951,16 @@
     </row>
     <row r="33" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B33" s="24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H33" s="27"/>
       <c r="I33" s="24" t="s">
@@ -7929,18 +7970,18 @@
     </row>
     <row r="34" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B34" s="24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="27"/>
       <c r="E34" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="24" t="s">
@@ -7950,16 +7991,16 @@
     </row>
     <row r="35" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B35" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="24" t="s">
@@ -7969,18 +8010,18 @@
     </row>
     <row r="36" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B36" s="24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="27"/>
       <c r="E36" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H36" s="27"/>
       <c r="I36" s="24" t="s">
@@ -7990,16 +8031,16 @@
     </row>
     <row r="37" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B37" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H37" s="27"/>
       <c r="I37" s="24" t="s">
@@ -8039,10 +8080,10 @@
       <c r="E41" s="62"/>
       <c r="F41" s="63"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="77" t="s">
+      <c r="H41" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="78"/>
+      <c r="I41" s="65"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
@@ -8051,22 +8092,22 @@
       <c r="D42" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="84"/>
-      <c r="F42" s="85"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="82"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="80"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="67"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
       <c r="C43" s="60"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="66"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="85"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="80"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="67"/>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8076,39 +8117,39 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="82"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="69"/>
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="9"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="72"/>
       <c r="G45" s="3"/>
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="73"/>
-      <c r="H46" s="67" t="s">
+      <c r="C46" s="73"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="75"/>
+      <c r="H46" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I46" s="67"/>
+      <c r="I46" s="79"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="73"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
       <c r="H47" s="28">
         <f>COUNTIF(I16:I38,"Pass")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -8120,10 +8161,10 @@
     </row>
     <row r="48" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="9"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="73"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="75"/>
       <c r="H48" s="28">
         <f>COUNTIF(I16:I38,"Fail")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -8135,10 +8176,10 @@
     </row>
     <row r="49" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="9"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="78"/>
       <c r="H49" s="28">
         <f>COUNTIF(I16:I38,"Not Run")/COUNTA(I16:I38)</f>
         <v>1</v>
@@ -8162,18 +8203,18 @@
     <row r="51" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="H41:I44"/>
     <mergeCell ref="D42:F43"/>
     <mergeCell ref="C45:F49"/>
     <mergeCell ref="H46:I46"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
     <cfRule type="cellIs" dxfId="83" priority="37" operator="equal">
@@ -8322,7 +8363,7 @@
   <dimension ref="B1:K51"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8362,10 +8403,10 @@
       <c r="E3" s="62"/>
       <c r="F3" s="63"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
@@ -8373,25 +8414,25 @@
       <c r="B4" s="9"/>
       <c r="C4" s="60"/>
       <c r="D4" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+        <v>353</v>
+      </c>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
       <c r="C5" s="60"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -8402,42 +8443,42 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="82"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
-      <c r="C7" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="C7" s="70" t="s">
+        <v>354</v>
+      </c>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
       <c r="J7" s="16"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73"/>
-      <c r="H8" s="67" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="H8" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="28">
         <f>COUNTIF(I16:I38,"Pass")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -8450,10 +8491,10 @@
     </row>
     <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="28">
         <f>COUNTIF(I16:I38,"Fail")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -8466,10 +8507,10 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="H11" s="28">
         <f>COUNTIF(I16:I38,"Not Run")/COUNTA(I16:I38)</f>
         <v>1</v>
@@ -8523,16 +8564,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="63" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="D16" s="26"/>
+        <v>326</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E16" s="24" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
@@ -8544,20 +8587,20 @@
     </row>
     <row r="17" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>333</v>
-      </c>
       <c r="G17" s="27" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="24" t="s">
@@ -8567,20 +8610,20 @@
     </row>
     <row r="18" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>333</v>
-      </c>
       <c r="G18" s="27" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="24" t="s">
@@ -8590,20 +8633,20 @@
     </row>
     <row r="19" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>333</v>
-      </c>
       <c r="G19" s="27" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="24" t="s">
@@ -8613,20 +8656,20 @@
     </row>
     <row r="20" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="F20" s="26" t="s">
-        <v>333</v>
-      </c>
       <c r="G20" s="27" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="24" t="s">
@@ -8636,20 +8679,22 @@
     </row>
     <row r="21" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>342</v>
-      </c>
-      <c r="D21" s="27"/>
+        <v>339</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>359</v>
+      </c>
       <c r="E21" s="53" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="24" t="s">
@@ -8865,34 +8910,35 @@
       <c r="E41" s="62"/>
       <c r="F41" s="63"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="77" t="s">
+      <c r="H41" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="78"/>
+      <c r="I41" s="65"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
       <c r="C42" s="60"/>
-      <c r="D42" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="E42" s="84"/>
-      <c r="F42" s="85"/>
+      <c r="D42" s="61" t="str">
+        <f>D4</f>
+        <v>3.5 FUNCTIONAL TEST CASES FOR USE CASE: USABILITY OF CALENDAR (EVENT PLOTTING)</v>
+      </c>
+      <c r="E42" s="81"/>
+      <c r="F42" s="82"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="80"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="67"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9"/>
       <c r="C43" s="60"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="66"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="85"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="80"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="67"/>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="2:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8902,41 +8948,41 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="82"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="69"/>
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="9"/>
-      <c r="C45" s="68" t="str">
+      <c r="C45" s="70" t="str">
         <f>C7</f>
         <v>Test Case validates the following: 
-• The links properly redirect the user to the necessary audio files / text files / websites</v>
-      </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="70"/>
+• The Event Plotting of all movable feasts and the completeness of all the readings per month</v>
+      </c>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="72"/>
       <c r="G45" s="3"/>
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="73"/>
-      <c r="H46" s="67" t="s">
+      <c r="C46" s="73"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="75"/>
+      <c r="H46" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I46" s="67"/>
+      <c r="I46" s="79"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="73"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
       <c r="H47" s="28">
         <f>COUNTIF(I16:I38,"Pass")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -8948,10 +8994,10 @@
     </row>
     <row r="48" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="9"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="73"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="75"/>
       <c r="H48" s="28">
         <f>COUNTIF(I16:I38,"Fail")/COUNTA(I16:I38)</f>
         <v>0</v>
@@ -8963,10 +9009,10 @@
     </row>
     <row r="49" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="9"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="78"/>
       <c r="H49" s="28">
         <f>COUNTIF(I16:I38,"Not Run")/COUNTA(I16:I38)</f>
         <v>1</v>
@@ -8990,18 +9036,18 @@
     <row r="51" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="D41:F41"/>
     <mergeCell ref="H41:I44"/>
     <mergeCell ref="D42:F43"/>
     <mergeCell ref="C45:F49"/>
     <mergeCell ref="H46:I46"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
     <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
@@ -9074,11 +9120,11 @@
   <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16:E76"/>
+      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9118,10 +9164,10 @@
       <c r="E3" s="62"/>
       <c r="F3" s="63"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
     </row>
@@ -9129,25 +9175,25 @@
       <c r="B4" s="9"/>
       <c r="C4" s="60"/>
       <c r="D4" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+        <v>61</v>
+      </c>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="16"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
       <c r="C5" s="60"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="17"/>
       <c r="K5" s="5"/>
     </row>
@@ -9158,42 +9204,42 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="82"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
-      <c r="C7" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="C7" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
       <c r="J7" s="16"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73"/>
-      <c r="H8" s="67" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="75"/>
+      <c r="H8" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="15"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="75"/>
       <c r="H9" s="28">
         <f>COUNTIF(I16:I37,"Pass")/COUNTA(I16:I37)</f>
         <v>0</v>
@@ -9206,10 +9252,10 @@
     </row>
     <row r="10" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
       <c r="H10" s="28">
         <f>COUNTIF(I16:I37,"Fail")/COUNTA(I16:I37)</f>
         <v>0</v>
@@ -9222,10 +9268,10 @@
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="H11" s="28">
         <f>COUNTIF(I16:I37,"Not Run")/COUNTA(I16:I37)</f>
         <v>1</v>
@@ -9281,20 +9327,22 @@
     </row>
     <row r="16" spans="2:11" ht="126" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" s="26"/>
+        <v>157</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>355</v>
+      </c>
       <c r="E16" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="27" t="s">
         <v>159</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>162</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="24" t="s">
@@ -9304,18 +9352,18 @@
     </row>
     <row r="17" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="27"/>
       <c r="E17" s="54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="24" t="s">
@@ -9325,16 +9373,16 @@
     </row>
     <row r="18" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="27"/>
       <c r="E18" s="54"/>
       <c r="F18" s="26" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="24" t="s">
@@ -9344,16 +9392,16 @@
     </row>
     <row r="19" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="27"/>
       <c r="E19" s="54"/>
       <c r="F19" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="24" t="s">
@@ -9363,16 +9411,16 @@
     </row>
     <row r="20" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="27"/>
       <c r="E20" s="55"/>
       <c r="F20" s="27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="24" t="s">
@@ -9382,16 +9430,16 @@
     </row>
     <row r="21" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="27"/>
       <c r="E21" s="54"/>
       <c r="F21" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="24" t="s">
@@ -9401,16 +9449,16 @@
     </row>
     <row r="22" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="27"/>
       <c r="E22" s="54"/>
       <c r="F22" s="26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="24" t="s">
@@ -9420,16 +9468,16 @@
     </row>
     <row r="23" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="27"/>
       <c r="E23" s="55"/>
       <c r="F23" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>175</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>178</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="24" t="s">
@@ -9439,16 +9487,16 @@
     </row>
     <row r="24" spans="2:10" ht="126" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="27"/>
       <c r="E24" s="55"/>
       <c r="F24" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="G24" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>179</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="24" t="s">
@@ -9458,16 +9506,16 @@
     </row>
     <row r="25" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="27"/>
       <c r="E25" s="55"/>
       <c r="F25" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="27" t="s">
         <v>177</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>180</v>
       </c>
       <c r="H25" s="27"/>
       <c r="I25" s="24" t="s">
@@ -9477,20 +9525,22 @@
     </row>
     <row r="26" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" s="27"/>
+        <v>178</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>356</v>
+      </c>
       <c r="E26" s="54" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="24" t="s">
@@ -9504,10 +9554,10 @@
       <c r="D27" s="27"/>
       <c r="E27" s="55"/>
       <c r="F27" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H27" s="27"/>
       <c r="I27" s="24" t="s">
@@ -9517,20 +9567,22 @@
     </row>
     <row r="28" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="G28" s="27" t="s">
         <v>187</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="55" t="s">
-        <v>159</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" s="27" t="s">
-        <v>190</v>
       </c>
       <c r="H28" s="27"/>
       <c r="I28" s="24" t="s">
@@ -9540,16 +9592,16 @@
     </row>
     <row r="29" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="27"/>
       <c r="E29" s="55"/>
       <c r="F29" s="27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H29" s="27"/>
       <c r="I29" s="24" t="s">
@@ -9559,18 +9611,18 @@
     </row>
     <row r="30" spans="2:10" ht="204.75" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="27"/>
       <c r="E30" s="55" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="24" t="s">
@@ -9580,20 +9632,22 @@
     </row>
     <row r="31" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="G31" s="27" t="s">
         <v>208</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="55" t="s">
-        <v>210</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>211</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="24" t="s">
@@ -9603,16 +9657,16 @@
     </row>
     <row r="32" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="27"/>
       <c r="E32" s="55"/>
       <c r="F32" s="27" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="24" t="s">
@@ -9622,16 +9676,16 @@
     </row>
     <row r="33" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="27"/>
       <c r="E33" s="55"/>
       <c r="F33" s="27" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H33" s="27"/>
       <c r="I33" s="24" t="s">
@@ -9641,20 +9695,22 @@
     </row>
     <row r="34" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="F34" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="G34" s="27" t="s">
         <v>219</v>
-      </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="54" t="s">
-        <v>220</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="G34" s="27" t="s">
-        <v>222</v>
       </c>
       <c r="H34" s="27"/>
       <c r="I34" s="24" t="s">
@@ -9664,16 +9720,16 @@
     </row>
     <row r="35" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="27"/>
       <c r="E35" s="55"/>
       <c r="F35" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="24" t="s">
@@ -9683,20 +9739,22 @@
     </row>
     <row r="36" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B36" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C36" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="55" t="s">
-        <v>220</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>226</v>
-      </c>
       <c r="G36" s="27" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H36" s="27"/>
       <c r="I36" s="24" t="s">
@@ -9706,16 +9764,16 @@
     </row>
     <row r="37" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B37" s="35" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
       <c r="E37" s="56"/>
       <c r="F37" s="36" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G37" s="36" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H37" s="36"/>
       <c r="I37" s="38" t="s">
@@ -9726,18 +9784,18 @@
     <row r="38" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A38" s="37"/>
       <c r="B38" s="42" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
       <c r="E38" s="57" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H38" s="37"/>
       <c r="I38" s="42" t="s">
@@ -9747,20 +9805,20 @@
     </row>
     <row r="39" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B39" s="48" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="55" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H39" s="37"/>
       <c r="I39" s="42" t="s">
@@ -9770,20 +9828,22 @@
     </row>
     <row r="40" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B40" s="52" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="D40" s="47"/>
+        <v>273</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>357</v>
+      </c>
       <c r="E40" s="56" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H40" s="47"/>
       <c r="I40" s="45" t="s">
@@ -9793,16 +9853,16 @@
     </row>
     <row r="41" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B41" s="42" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="37"/>
       <c r="E41" s="57"/>
       <c r="F41" s="41" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H41" s="37"/>
       <c r="I41" s="45" t="s">
@@ -9812,16 +9872,16 @@
     </row>
     <row r="42" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B42" s="52" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="37"/>
       <c r="E42" s="57"/>
       <c r="F42" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H42" s="37"/>
       <c r="I42" s="45" t="s">
@@ -9831,20 +9891,22 @@
     </row>
     <row r="43" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B43" s="52" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="D43" s="26"/>
+        <v>228</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>356</v>
+      </c>
       <c r="E43" s="54" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="24" t="s">
@@ -9854,16 +9916,16 @@
     </row>
     <row r="44" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B44" s="52" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="27"/>
       <c r="E44" s="55"/>
       <c r="F44" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H44" s="27"/>
       <c r="I44" s="24" t="s">
@@ -9873,20 +9935,22 @@
     </row>
     <row r="45" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B45" s="52" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D45" s="27"/>
+        <v>226</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>358</v>
+      </c>
       <c r="E45" s="55" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F45" s="36" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G45" s="36" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H45" s="27"/>
       <c r="I45" s="24" t="s">
@@ -9896,20 +9960,22 @@
     </row>
     <row r="46" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B46" s="52" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="D46" s="49"/>
+        <v>279</v>
+      </c>
+      <c r="D46" s="49" t="s">
+        <v>355</v>
+      </c>
       <c r="E46" s="55" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H46" s="37"/>
       <c r="I46" s="42" t="s">
@@ -9919,20 +9985,22 @@
     </row>
     <row r="47" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B47" s="52" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>285</v>
-      </c>
-      <c r="D47" s="47"/>
+        <v>282</v>
+      </c>
+      <c r="D47" s="47" t="s">
+        <v>357</v>
+      </c>
       <c r="E47" s="56" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F47" s="36" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G47" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H47" s="47"/>
       <c r="I47" s="45" t="s">
@@ -9942,16 +10010,16 @@
     </row>
     <row r="48" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B48" s="52" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="37"/>
       <c r="E48" s="57"/>
       <c r="F48" s="41" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G48" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H48" s="37"/>
       <c r="I48" s="45" t="s">
@@ -9961,16 +10029,16 @@
     </row>
     <row r="49" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B49" s="52" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="37"/>
       <c r="E49" s="57"/>
       <c r="F49" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H49" s="37"/>
       <c r="I49" s="45" t="s">
@@ -9980,20 +10048,22 @@
     </row>
     <row r="50" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B50" s="52" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C50" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="E50" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="G50" s="27" t="s">
         <v>240</v>
-      </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="54" t="s">
-        <v>241</v>
-      </c>
-      <c r="F50" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="G50" s="27" t="s">
-        <v>243</v>
       </c>
       <c r="H50" s="27"/>
       <c r="I50" s="42" t="s">
@@ -10003,16 +10073,16 @@
     </row>
     <row r="51" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B51" s="52" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C51" s="25"/>
       <c r="D51" s="27"/>
       <c r="E51" s="55"/>
       <c r="F51" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H51" s="27"/>
       <c r="I51" s="42" t="s">
@@ -10022,20 +10092,22 @@
     </row>
     <row r="52" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B52" s="52" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="D52" s="27"/>
+        <v>241</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>358</v>
+      </c>
       <c r="E52" s="55" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F52" s="27" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H52" s="27"/>
       <c r="I52" s="42" t="s">
@@ -10045,16 +10117,16 @@
     </row>
     <row r="53" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B53" s="52" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C53" s="35"/>
       <c r="D53" s="36"/>
       <c r="E53" s="55"/>
       <c r="F53" s="27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H53" s="27"/>
       <c r="I53" s="42" t="s">
@@ -10064,18 +10136,18 @@
     </row>
     <row r="54" spans="2:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B54" s="52" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="37"/>
       <c r="E54" s="58" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F54" s="27" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I54" s="42" t="s">
         <v>4</v>
@@ -10084,20 +10156,22 @@
     </row>
     <row r="55" spans="2:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B55" s="52" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C55" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D55" s="49" t="s">
+        <v>355</v>
+      </c>
+      <c r="E55" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="F55" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="G55" s="27" t="s">
         <v>288</v>
-      </c>
-      <c r="D55" s="49"/>
-      <c r="E55" s="55" t="s">
-        <v>241</v>
-      </c>
-      <c r="F55" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G55" s="27" t="s">
-        <v>291</v>
       </c>
       <c r="H55" s="37"/>
       <c r="I55" s="42" t="s">
@@ -10107,20 +10181,22 @@
     </row>
     <row r="56" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B56" s="52" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C56" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="D56" s="47" t="s">
+        <v>357</v>
+      </c>
+      <c r="E56" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="D56" s="47"/>
-      <c r="E56" s="56" t="s">
-        <v>292</v>
-      </c>
       <c r="F56" s="36" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G56" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H56" s="47"/>
       <c r="I56" s="45" t="s">
@@ -10130,16 +10206,16 @@
     </row>
     <row r="57" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B57" s="52" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="37"/>
       <c r="E57" s="57"/>
       <c r="F57" s="41" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G57" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H57" s="37"/>
       <c r="I57" s="45" t="s">
@@ -10149,16 +10225,16 @@
     </row>
     <row r="58" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B58" s="52" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="37"/>
       <c r="E58" s="57"/>
       <c r="F58" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H58" s="37"/>
       <c r="I58" s="45" t="s">
@@ -10168,20 +10244,22 @@
     </row>
     <row r="59" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B59" s="52" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C59" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="E59" s="54" t="s">
+        <v>248</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="G59" s="27" t="s">
         <v>250</v>
-      </c>
-      <c r="D59" s="27"/>
-      <c r="E59" s="54" t="s">
-        <v>251</v>
-      </c>
-      <c r="F59" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="G59" s="27" t="s">
-        <v>253</v>
       </c>
       <c r="H59" s="27"/>
       <c r="I59" s="42" t="s">
@@ -10191,16 +10269,16 @@
     </row>
     <row r="60" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B60" s="52" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C60" s="25"/>
       <c r="D60" s="27"/>
       <c r="E60" s="55"/>
       <c r="F60" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G60" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H60" s="27"/>
       <c r="I60" s="42" t="s">
@@ -10210,20 +10288,22 @@
     </row>
     <row r="61" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B61" s="52" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="D61" s="27"/>
+        <v>251</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>358</v>
+      </c>
       <c r="E61" s="55" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F61" s="27" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G61" s="27" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H61" s="27"/>
       <c r="I61" s="42" t="s">
@@ -10233,16 +10313,16 @@
     </row>
     <row r="62" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B62" s="52" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C62" s="35"/>
       <c r="D62" s="36"/>
       <c r="E62" s="55"/>
       <c r="F62" s="27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G62" s="27" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H62" s="27"/>
       <c r="I62" s="42" t="s">
@@ -10252,18 +10332,18 @@
     </row>
     <row r="63" spans="2:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B63" s="52" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="37"/>
       <c r="E63" s="58" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F63" s="27" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I63" s="42" t="s">
         <v>4</v>
@@ -10272,20 +10352,22 @@
     </row>
     <row r="64" spans="2:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B64" s="52" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>300</v>
-      </c>
-      <c r="D64" s="49"/>
+        <v>297</v>
+      </c>
+      <c r="D64" s="49" t="s">
+        <v>355</v>
+      </c>
       <c r="E64" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="G64" s="27" t="s">
         <v>302</v>
-      </c>
-      <c r="F64" s="27" t="s">
-        <v>304</v>
-      </c>
-      <c r="G64" s="27" t="s">
-        <v>305</v>
       </c>
       <c r="H64" s="37"/>
       <c r="I64" s="42" t="s">
@@ -10295,20 +10377,22 @@
     </row>
     <row r="65" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B65" s="52" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>301</v>
-      </c>
-      <c r="D65" s="47"/>
+        <v>298</v>
+      </c>
+      <c r="D65" s="47" t="s">
+        <v>357</v>
+      </c>
       <c r="E65" s="56" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F65" s="36" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G65" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H65" s="47"/>
       <c r="I65" s="45" t="s">
@@ -10318,16 +10402,16 @@
     </row>
     <row r="66" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B66" s="52" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C66" s="42"/>
       <c r="D66" s="37"/>
       <c r="E66" s="57"/>
       <c r="F66" s="41" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G66" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H66" s="37"/>
       <c r="I66" s="45" t="s">
@@ -10337,16 +10421,16 @@
     </row>
     <row r="67" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B67" s="52" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="37"/>
       <c r="E67" s="57"/>
       <c r="F67" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H67" s="37"/>
       <c r="I67" s="45" t="s">
@@ -10356,20 +10440,22 @@
     </row>
     <row r="68" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B68" s="52" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C68" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="E68" s="54" t="s">
+        <v>262</v>
+      </c>
+      <c r="F68" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="G68" s="27" t="s">
         <v>264</v>
-      </c>
-      <c r="D68" s="27"/>
-      <c r="E68" s="54" t="s">
-        <v>265</v>
-      </c>
-      <c r="F68" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="G68" s="27" t="s">
-        <v>267</v>
       </c>
       <c r="H68" s="27"/>
       <c r="I68" s="42" t="s">
@@ -10379,16 +10465,16 @@
     </row>
     <row r="69" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B69" s="52" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="27"/>
       <c r="E69" s="55"/>
       <c r="F69" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G69" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H69" s="27"/>
       <c r="I69" s="42" t="s">
@@ -10398,20 +10484,22 @@
     </row>
     <row r="70" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B70" s="52" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="D70" s="27"/>
+        <v>265</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>358</v>
+      </c>
       <c r="E70" s="55" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F70" s="27" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H70" s="27"/>
       <c r="I70" s="42" t="s">
@@ -10421,16 +10509,16 @@
     </row>
     <row r="71" spans="2:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B71" s="52" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C71" s="35"/>
       <c r="D71" s="36"/>
       <c r="E71" s="56"/>
       <c r="F71" s="36" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G71" s="36" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H71" s="36"/>
       <c r="I71" s="45" t="s">
@@ -10440,18 +10528,18 @@
     </row>
     <row r="72" spans="2:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B72" s="52" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="37"/>
       <c r="E72" s="57" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G72" s="41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H72" s="37"/>
       <c r="I72" s="42" t="s">
@@ -10461,20 +10549,22 @@
     </row>
     <row r="73" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B73" s="52" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C73" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D73" s="49" t="s">
+        <v>355</v>
+      </c>
+      <c r="E73" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="F73" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="D73" s="49"/>
-      <c r="E73" s="55" t="s">
-        <v>265</v>
-      </c>
-      <c r="F73" s="27" t="s">
-        <v>318</v>
-      </c>
       <c r="G73" s="27" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H73" s="37"/>
       <c r="I73" s="42" t="s">
@@ -10484,20 +10574,22 @@
     </row>
     <row r="74" spans="2:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B74" s="52" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C74" s="35" t="s">
-        <v>316</v>
-      </c>
-      <c r="D74" s="47"/>
+        <v>313</v>
+      </c>
+      <c r="D74" s="47" t="s">
+        <v>357</v>
+      </c>
       <c r="E74" s="56" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F74" s="36" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G74" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H74" s="47"/>
       <c r="I74" s="45" t="s">
@@ -10507,16 +10599,16 @@
     </row>
     <row r="75" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B75" s="52" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C75" s="42"/>
       <c r="D75" s="37"/>
       <c r="E75" s="57"/>
       <c r="F75" s="41" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G75" s="41" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H75" s="37"/>
       <c r="I75" s="45" t="s">
@@ -10526,16 +10618,16 @@
     </row>
     <row r="76" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B76" s="52" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C76" s="42"/>
       <c r="D76" s="37"/>
       <c r="E76" s="57"/>
       <c r="F76" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G76" s="27" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H76" s="37"/>
       <c r="I76" s="45" t="s">
@@ -10605,34 +10697,34 @@
       <c r="E82" s="62"/>
       <c r="F82" s="63"/>
       <c r="G82" s="14"/>
-      <c r="H82" s="77" t="s">
+      <c r="H82" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I82" s="78"/>
+      <c r="I82" s="65"/>
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="60"/>
       <c r="D83" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="E83" s="84"/>
-      <c r="F83" s="85"/>
+        <v>61</v>
+      </c>
+      <c r="E83" s="81"/>
+      <c r="F83" s="82"/>
       <c r="G83" s="3"/>
-      <c r="H83" s="79"/>
-      <c r="I83" s="80"/>
+      <c r="H83" s="66"/>
+      <c r="I83" s="67"/>
       <c r="J83" s="16"/>
     </row>
     <row r="84" spans="2:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="9"/>
       <c r="C84" s="60"/>
-      <c r="D84" s="64"/>
-      <c r="E84" s="65"/>
-      <c r="F84" s="66"/>
+      <c r="D84" s="83"/>
+      <c r="E84" s="84"/>
+      <c r="F84" s="85"/>
       <c r="G84" s="5"/>
-      <c r="H84" s="79"/>
-      <c r="I84" s="80"/>
+      <c r="H84" s="66"/>
+      <c r="I84" s="67"/>
       <c r="J84" s="17"/>
     </row>
     <row r="85" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -10642,39 +10734,39 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="81"/>
-      <c r="I85" s="82"/>
+      <c r="H85" s="68"/>
+      <c r="I85" s="69"/>
       <c r="J85" s="10"/>
     </row>
     <row r="86" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="9"/>
-      <c r="C86" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="D86" s="69"/>
-      <c r="E86" s="69"/>
-      <c r="F86" s="70"/>
+      <c r="C86" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="D86" s="71"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="72"/>
       <c r="G86" s="3"/>
       <c r="J86" s="16"/>
     </row>
     <row r="87" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="9"/>
-      <c r="C87" s="71"/>
-      <c r="D87" s="72"/>
-      <c r="E87" s="72"/>
-      <c r="F87" s="73"/>
-      <c r="H87" s="67" t="s">
+      <c r="C87" s="73"/>
+      <c r="D87" s="74"/>
+      <c r="E87" s="74"/>
+      <c r="F87" s="75"/>
+      <c r="H87" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I87" s="67"/>
+      <c r="I87" s="79"/>
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="9"/>
-      <c r="C88" s="71"/>
-      <c r="D88" s="72"/>
-      <c r="E88" s="72"/>
-      <c r="F88" s="73"/>
+      <c r="C88" s="73"/>
+      <c r="D88" s="74"/>
+      <c r="E88" s="74"/>
+      <c r="F88" s="75"/>
       <c r="H88" s="28">
         <f>COUNTIF(I16:I37,"Pass")/COUNTA(I16:I37)</f>
         <v>0</v>
@@ -10686,10 +10778,10 @@
     </row>
     <row r="89" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="9"/>
-      <c r="C89" s="71"/>
-      <c r="D89" s="72"/>
-      <c r="E89" s="72"/>
-      <c r="F89" s="73"/>
+      <c r="C89" s="73"/>
+      <c r="D89" s="74"/>
+      <c r="E89" s="74"/>
+      <c r="F89" s="75"/>
       <c r="H89" s="28">
         <f>COUNTIF(I16:I37,"Fail")/COUNTA(I16:I37)</f>
         <v>0</v>
@@ -10701,10 +10793,10 @@
     </row>
     <row r="90" spans="2:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="9"/>
-      <c r="C90" s="74"/>
-      <c r="D90" s="75"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="76"/>
+      <c r="C90" s="76"/>
+      <c r="D90" s="77"/>
+      <c r="E90" s="77"/>
+      <c r="F90" s="78"/>
       <c r="H90" s="28">
         <f>COUNTIF(I16:I37,"Not Run")/COUNTA(I16:I37)</f>
         <v>1</v>
@@ -10728,18 +10820,18 @@
     <row r="92" spans="2:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H3:I6"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="C7:F11"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="D82:F82"/>
     <mergeCell ref="H82:I85"/>
     <mergeCell ref="D83:F84"/>
     <mergeCell ref="C86:F90"/>
     <mergeCell ref="H87:I87"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:I6"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="C7:F11"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I11">
     <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">

</xml_diff>